<commit_message>
MN | Additional xls file for reporting download
</commit_message>
<xml_diff>
--- a/application/download/pws1.xlsx
+++ b/application/download/pws1.xlsx
@@ -240,7 +240,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +253,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -346,19 +352,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -387,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,24 +423,24 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -469,33 +462,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,8 +795,8 @@
   </sheetPr>
   <dimension ref="A1:AMK60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1024,38 +1018,38 @@
       <c r="AD6" s="8"/>
     </row>
     <row r="7" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="47" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="47" t="s">
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="47" t="s">
+      <c r="M7" s="51"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -1068,56 +1062,56 @@
       <c r="AD7" s="8"/>
     </row>
     <row r="8" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="43" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45" t="s">
+      <c r="K8" s="50"/>
+      <c r="L8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="45" t="s">
+      <c r="N8" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="46" t="s">
+      <c r="O8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="45" t="s">
+      <c r="P8" s="50"/>
+      <c r="Q8" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="45" t="s">
+      <c r="R8" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="46" t="s">
+      <c r="S8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="44"/>
+      <c r="T8" s="50"/>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
@@ -1130,32 +1124,32 @@
       <c r="AD8" s="8"/>
     </row>
     <row r="9" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="44"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="50"/>
       <c r="O9" s="18" t="s">
         <v>20</v>
       </c>
       <c r="P9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="50"/>
       <c r="S9" s="18" t="s">
         <v>20</v>
       </c>
@@ -1174,62 +1168,62 @@
       <c r="AD9" s="8"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
+      <c r="A10" s="52">
         <v>1</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="52">
         <v>2</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="52">
         <v>3</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19">
+      <c r="D10" s="52"/>
+      <c r="E10" s="52">
         <v>4</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="52">
         <v>5</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="53">
         <v>7</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="53">
         <v>8</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="53">
         <v>9</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="53">
         <v>10</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="53">
         <v>11</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="53">
         <v>12</v>
       </c>
-      <c r="M10" s="20">
+      <c r="M10" s="53">
         <v>13</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="53">
         <v>14</v>
       </c>
-      <c r="O10" s="20">
+      <c r="O10" s="53">
         <v>15</v>
       </c>
-      <c r="P10" s="20">
+      <c r="P10" s="53">
         <v>16</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="53">
         <v>17</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="53">
         <v>18</v>
       </c>
-      <c r="S10" s="20">
+      <c r="S10" s="53">
         <v>20</v>
       </c>
-      <c r="T10" s="20">
+      <c r="T10" s="53">
         <v>21</v>
       </c>
       <c r="U10" s="8"/>
@@ -1258,7 +1252,7 @@
         <v>190</v>
       </c>
       <c r="F11" s="19"/>
-      <c r="G11" s="50">
+      <c r="G11" s="43">
         <v>4</v>
       </c>
       <c r="H11" s="20"/>
@@ -1322,7 +1316,7 @@
         <v>78</v>
       </c>
       <c r="F12" s="19"/>
-      <c r="G12" s="50">
+      <c r="G12" s="43">
         <v>31</v>
       </c>
       <c r="H12" s="20"/>
@@ -1388,7 +1382,7 @@
         <v>214</v>
       </c>
       <c r="F13" s="19"/>
-      <c r="G13" s="50">
+      <c r="G13" s="43">
         <v>13</v>
       </c>
       <c r="H13" s="20" t="s">
@@ -1520,7 +1514,7 @@
         <v>220</v>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="50">
+      <c r="G15" s="43">
         <v>94</v>
       </c>
       <c r="H15" s="20" t="s">
@@ -1590,7 +1584,7 @@
         <v>161</v>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="50">
+      <c r="G16" s="43">
         <v>21</v>
       </c>
       <c r="H16" s="20" t="s">
@@ -1660,7 +1654,7 @@
         <v>211</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="50">
+      <c r="G17" s="43">
         <v>29</v>
       </c>
       <c r="H17" s="20"/>
@@ -1726,7 +1720,7 @@
         <v>190</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="50">
+      <c r="G18" s="43">
         <v>6</v>
       </c>
       <c r="H18" s="20"/>
@@ -1792,7 +1786,7 @@
         <v>69</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="50">
+      <c r="G19" s="43">
         <v>27</v>
       </c>
       <c r="H19" s="20" t="s">
@@ -1860,7 +1854,7 @@
         <v>247</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="50">
+      <c r="G20" s="43">
         <v>11</v>
       </c>
       <c r="H20" s="20"/>
@@ -1926,7 +1920,7 @@
         <v>81</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="50">
+      <c r="G21" s="43">
         <v>36</v>
       </c>
       <c r="H21" s="20"/>
@@ -2140,34 +2134,34 @@
       <c r="AD24" s="8"/>
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="51">
+      <c r="B25" s="47"/>
+      <c r="C25" s="44">
         <f>SUM(C24:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="51">
+      <c r="D25" s="44">
         <f>SUM(D24:D24)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="44">
         <f>SUM(E24:E24)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51">
+      <c r="F25" s="44"/>
+      <c r="G25" s="44">
         <f>SUM(G11:G24)</f>
         <v>272</v>
       </c>
-      <c r="H25" s="51"/>
-      <c r="I25" s="52">
+      <c r="H25" s="44"/>
+      <c r="I25" s="45">
         <f>96/12*1</f>
         <v>8</v>
       </c>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52" t="e">
+      <c r="J25" s="44"/>
+      <c r="K25" s="45" t="e">
         <f>J25/C25*100</f>
         <v>#DIV/0!</v>
       </c>
@@ -2597,6 +2591,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:P7"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="Q7:T7"/>
     <mergeCell ref="C8:C9"/>
@@ -2613,12 +2613,6 @@
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:P7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>